<commit_message>
Calibrated pressure using bme280 and added +50 to value in analog.py
</commit_message>
<xml_diff>
--- a/data/calbration_vertical_factor.xlsx
+++ b/data/calbration_vertical_factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c6e372e5b8c96f59/stom/systems/vacuum_meter/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mh/OneDrive/stom/systems/vacuum_meter/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:4000b_{30BB89E4-3CEC-0C4C-A1F1-C46149648F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:4000b_{DAA0F178-E61E-8149-B375-58A34138C728}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2F13E7F7-C71C-F746-976D-2001DCAD93F1}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calbration_vertical_factor" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>timestamp</t>
   </si>
@@ -231,14 +253,17 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="179" formatCode="0.00000000000000000000"/>
+    <numFmt numFmtId="173" formatCode="0.000000000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -719,7 +744,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -765,9 +790,15 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="179" formatCode="0.00000000000000000000"/>
+      <numFmt numFmtId="173" formatCode="0.000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode="0.000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode="0.000000000000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -783,29 +814,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B64" totalsRowShown="0">
-  <autoFilter ref="A1:B64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B64" totalsRowShown="0">
+  <autoFilter ref="A1:B64" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B64">
     <sortCondition ref="B1:B64"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="timestamp"/>
-    <tableColumn id="2" name="load"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="timestamp"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="load"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="H9:I10" totalsRowShown="0">
-  <autoFilter ref="H9:I10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="H9:I10" totalsRowShown="0">
+  <autoFilter ref="H9:I10" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Reference"/>
-    <tableColumn id="2" name="Average" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Reference"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Average" dataDxfId="2">
       <calculatedColumnFormula>AVERAGE(B:B)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2CA712AC-A7AC-9043-972D-90C98048A101}" name="Table3" displayName="Table3" ref="H14:H15" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="H14:H15" xr:uid="{01524A70-D2FF-1C40-97B2-621069693CFF}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{1D5E8B69-9458-C649-A1D6-A91C17415264}" name="C" dataDxfId="1">
+      <calculatedColumnFormula array="1">Table2[Average]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1105,18 +1148,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1243,6 +1286,9 @@
       <c r="B14">
         <v>-157.12477628072401</v>
       </c>
+      <c r="H14" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1251,6 +1297,10 @@
       <c r="B15">
         <v>-156.94888220735001</v>
       </c>
+      <c r="H15" s="1" cm="1">
+        <f t="array" ref="H15">Table2[Average]</f>
+        <v>-155.78750048390086</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1646,9 +1696,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>